<commit_message>
Cleaned price values before saving to Excel
</commit_message>
<xml_diff>
--- a/amazon_watches.xlsx
+++ b/amazon_watches.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D141"/>
+  <dimension ref="A1:D127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,7 +512,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1,999</t>
+          <t>1999</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -534,7 +534,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1,999</t>
+          <t>1999</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -546,17 +546,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Sonata</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Quartz Multifunction Green Dial Green Leather Strap Watch for Men</t>
+          <t>Bold Quartz Analog Black Dial Silver Stainless Steel Strap Watch for Guys - NT38051SM07</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2,495</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -568,17 +568,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Sonata</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Quartz Multifunction Green Dial Green Leather Strap Watch for Men</t>
+          <t>Bold Quartz Analog Black Dial Silver Stainless Steel Strap Watch for Guys - NT38051SM07</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2,495</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -590,17 +590,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Titan</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Titan Metal Maritime Analog Grey Dial Men's Watch Nm1830Km01/Nn1830Km01, Band Color-Grey</t>
+          <t>Fastrack Stunners Quartz Analog Blue Dial Silver Metal Strap Watch for Guys - 3278SM03</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>16,406</t>
+          <t>1495</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -612,17 +612,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Titan</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Titan Metal Maritime Analog Grey Dial Men's Watch Nm1830Km01/Nn1830Km01, Band Color-Grey</t>
+          <t>Fastrack Stunners Quartz Analog Blue Dial Silver Metal Strap Watch for Guys - 3278SM03</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>16,406</t>
+          <t>1495</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -634,17 +634,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Noise</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Bold Quartz Analog Black Dial Silver Stainless Steel Strap Watch for Guys - NT38051SM07</t>
+          <t>Noise Twist Round dial Smart Watch with Bluetooth Calling, 1.38" TFT Display, up-to 7 Days Battery, 100+ Watch Faces, IP68, Heart Rate Monitor, Sleep Tracking (Jet Black)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1,995</t>
+          <t>1399</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -656,17 +656,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Noise</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Bold Quartz Analog Black Dial Silver Stainless Steel Strap Watch for Guys - NT38051SM07</t>
+          <t>Noise Twist Round dial Smart Watch with Bluetooth Calling, 1.38" TFT Display, up-to 7 Days Battery, 100+ Watch Faces, IP68, Heart Rate Monitor, Sleep Tracking (Jet Black)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1,995</t>
+          <t>1399</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -678,17 +678,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Titan</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Fastrack Stunners Quartz Analog Blue Dial Silver Metal Strap Watch for Guys - 3278SM03</t>
+          <t>Titan Neo Iv Analog Silver Dial Men's Watch-1802SL02 / 1802SL02</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1,495</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -700,17 +700,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Titan</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Fastrack Stunners Quartz Analog Blue Dial Silver Metal Strap Watch for Guys - 3278SM03</t>
+          <t>Titan Neo Iv Analog Silver Dial Men's Watch-1802SL02 / 1802SL02</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1,495</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -722,17 +722,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Noise</t>
+          <t>Titan</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Noise Twist Round dial Smart Watch with Bluetooth Calling, 1.38" TFT Display, up-to 7 Days Battery, 100+ Watch Faces, IP68, Heart Rate Monitor, Sleep Tracking (Jet Black)</t>
+          <t>Karishma Analog Multi-Colour Dial Men's Watch NM1639SM01/NN1639SM01</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1,399</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -744,17 +744,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Noise</t>
+          <t>Titan</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Noise Twist Round dial Smart Watch with Bluetooth Calling, 1.38" TFT Display, up-to 7 Days Battery, 100+ Watch Faces, IP68, Heart Rate Monitor, Sleep Tracking (Jet Black)</t>
+          <t>Karishma Analog Multi-Colour Dial Men's Watch NM1639SM01/NN1639SM01</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>1,399</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -766,17 +766,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Titan</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Titan Neo Iv Analog Silver Dial Men's Watch-1802SL02 / 1802SL02</t>
+          <t>Trendies Analog Black Dial Men's Watch-38058PP03/NP38058PP03</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1,995</t>
+          <t>1595</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -788,17 +788,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Titan</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Titan Neo Iv Analog Silver Dial Men's Watch-1802SL02 / 1802SL02</t>
+          <t>Trendies Analog Black Dial Men's Watch-38058PP03/NP38058PP03</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1,995</t>
+          <t>1595</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -810,17 +810,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Titan</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Karishma Analog Multi-Colour Dial Men's Watch NM1639SM01/NN1639SM01</t>
+          <t>Fastrack Limitless Glide X 1.83" Smart Watch with Ultra UV HD Display, SpO2, Heart Rate &amp; Sleep Tracking, Bluetooth Calling, 100+ Sports Modes, 5-Day Battery, Smartwatch for Men &amp; Women (Blue)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1,995</t>
+          <t>1499</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -832,17 +832,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Titan</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Karishma Analog Multi-Colour Dial Men's Watch NM1639SM01/NN1639SM01</t>
+          <t>Fastrack Limitless Glide X 1.83" Smart Watch with Ultra UV HD Display, SpO2, Heart Rate &amp; Sleep Tracking, Bluetooth Calling, 100+ Sports Modes, 5-Day Battery, Smartwatch for Men &amp; Women (Blue)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1,995</t>
+          <t>1499</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -854,17 +854,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Carlington</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Trendies Analog Black Dial Men's Watch-38058PP03/NP38058PP03</t>
+          <t>Endurance Series Analog-Digital Sports Watches for Men and Boys with Alarm, Stopwatch, Backlit Display, Dualtime, Silicone Rubber Strap, Water &amp; Shock Resiatant - CT_9105</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1,595</t>
+          <t>1299</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -876,17 +876,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Carlington</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Trendies Analog Black Dial Men's Watch-38058PP03/NP38058PP03</t>
+          <t>Endurance Series Analog-Digital Sports Watches for Men and Boys with Alarm, Stopwatch, Backlit Display, Dualtime, Silicone Rubber Strap, Water &amp; Shock Resiatant - CT_9105</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1,595</t>
+          <t>1299</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -898,17 +898,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Carlington</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Fastrack Limitless Glide X 1.83" Smart Watch with Ultra UV HD Display, SpO2, Heart Rate &amp; Sleep Tracking, Bluetooth Calling, 100+ Sports Modes, 5-Day Battery, Smartwatch for Men &amp; Women (Blue)</t>
+          <t>Stainless Steel Analog Wrist Watches for Men-Ct 8822</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1,499</t>
+          <t>1799</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -920,17 +920,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Carlington</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Fastrack Limitless Glide X 1.83" Smart Watch with Ultra UV HD Display, SpO2, Heart Rate &amp; Sleep Tracking, Bluetooth Calling, 100+ Sports Modes, 5-Day Battery, Smartwatch for Men &amp; Women (Blue)</t>
+          <t>Stainless Steel Analog Wrist Watches for Men-Ct 8822</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1,499</t>
+          <t>1799</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -942,17 +942,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Carlington</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Endurance Series Analog-Digital Sports Watches for Men and Boys with Alarm, Stopwatch, Backlit Display, Dualtime, Silicone Rubber Strap, Water &amp; Shock Resiatant - CT_9105</t>
+          <t>Bold Analog White Dial Men's Watch NM38051SL06/NN38051SL06</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1,299</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -964,17 +964,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Carlington</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Endurance Series Analog-Digital Sports Watches for Men and Boys with Alarm, Stopwatch, Backlit Display, Dualtime, Silicone Rubber Strap, Water &amp; Shock Resiatant - CT_9105</t>
+          <t>Bold Analog White Dial Men's Watch NM38051SL06/NN38051SL06</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1,299</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -986,17 +986,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Carlington</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Stainless Steel Analog Wrist Watches for Men-Ct 8822</t>
+          <t>Fastrack Vyb Quartz Analog Black Dial Black Genuine Leather Strap Watch for Men-FV30011NL01W</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1,799</t>
+          <t>1494</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1008,17 +1008,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Carlington</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Stainless Steel Analog Wrist Watches for Men-Ct 8822</t>
+          <t>Fastrack Vyb Quartz Analog Black Dial Black Genuine Leather Strap Watch for Men-FV30011NL01W</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1,799</t>
+          <t>1494</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1035,12 +1035,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Bold Analog White Dial Men's Watch NM38051SL06/NN38051SL06</t>
+          <t>Fastrack Vyb Maverick Quartz Analog Black Dial Watch for Men</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1,995</t>
+          <t>1893</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1057,12 +1057,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Bold Analog White Dial Men's Watch NM38051SL06/NN38051SL06</t>
+          <t>Fastrack Vyb Maverick Quartz Analog Black Dial Watch for Men</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1,995</t>
+          <t>1893</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1074,17 +1074,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Casio</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Fastrack Vyb Quartz Analog Black Dial Black Genuine Leather Strap Watch for Men-FV30011NL01W</t>
+          <t>Youth Series Digital Black Dial Unisex Watch - F-91W-1Q(D002)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1,494</t>
+          <t>1295</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1096,17 +1096,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Casio</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Fastrack Vyb Quartz Analog Black Dial Black Genuine Leather Strap Watch for Men-FV30011NL01W</t>
+          <t>Youth Series Digital Black Dial Unisex Watch - F-91W-1Q(D002)</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1,494</t>
+          <t>1295</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1118,17 +1118,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Noise</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Fastrack Vyb Maverick Quartz Analog Black Dial Watch for Men</t>
+          <t>Noise Twist Go Round dial Smartwatch with BT Calling, 1.39" Display, Metal Build, 100+ Watch Faces, IP68, Sleep Tracking, 100+ Sports Modes, 24/7 Heart Rate Monitoring (Elite Black)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1,893</t>
+          <t>1799</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1140,17 +1140,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Noise</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Fastrack Vyb Maverick Quartz Analog Black Dial Watch for Men</t>
+          <t>Noise Twist Go Round dial Smartwatch with BT Calling, 1.39" Display, Metal Build, 100+ Watch Faces, IP68, Sleep Tracking, 100+ Sports Modes, 24/7 Heart Rate Monitoring (Elite Black)</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1,893</t>
+          <t>1799</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1162,17 +1162,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Casio</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Youth Series Digital Black Dial Unisex Watch - F-91W-1Q(D002)</t>
+          <t>Fastrack Volt S1 Smart Watch for Man and Women Latest with 1.83" Display, Silicone Strap, BT Calling, 100+ Sports Modes, Heart Rate, SpO2, IP68, Ideal Smartwatch for Boys and Girls (Wine Red)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1,295</t>
+          <t>1499</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1184,17 +1184,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Casio</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Youth Series Digital Black Dial Unisex Watch - F-91W-1Q(D002)</t>
+          <t>Fastrack Volt S1 Smart Watch for Man and Women Latest with 1.83" Display, Silicone Strap, BT Calling, 100+ Sports Modes, Heart Rate, SpO2, IP68, Ideal Smartwatch for Boys and Girls (Wine Red)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1,295</t>
+          <t>1499</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1206,17 +1206,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Noise</t>
+          <t>Fire-Boltt</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Noise Twist Go Round dial Smartwatch with BT Calling, 1.39" Display, Metal Build, 100+ Watch Faces, IP68, Sleep Tracking, 100+ Sports Modes, 24/7 Heart Rate Monitoring (Elite Black)</t>
+          <t>Fire-Boltt Phoenix Smart Watch with Bluetooth Calling 1.38,120+ Sports Modes, 240 * 240 PX High Res with SpO2, Heart Rate Monitoring &amp; IP67 Rating (Black)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>1,799</t>
+          <t>1199</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1228,17 +1228,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Noise</t>
+          <t>Fire-Boltt</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Noise Twist Go Round dial Smartwatch with BT Calling, 1.39" Display, Metal Build, 100+ Watch Faces, IP68, Sleep Tracking, 100+ Sports Modes, 24/7 Heart Rate Monitoring (Elite Black)</t>
+          <t>Fire-Boltt Phoenix Smart Watch with Bluetooth Calling 1.38,120+ Sports Modes, 240 * 240 PX High Res with SpO2, Heart Rate Monitoring &amp; IP67 Rating (Black)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1,799</t>
+          <t>1199</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1250,17 +1250,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Fire-Boltt</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Fastrack Astor FR2 Pro 1.43" AMOLED Stainless Steel Smart Watch with SpO2, Heart Rate, BT Calling, Adaptive AOD, Functional Crown, AI Voice Assistant – Smartwatch for Stylish Professionals (Black)</t>
+          <t>Fire-Boltt Phoenix Ultra Luxury Stainless Steel, Bluetooth Calling Smart Watch, AI Voice Assistant, Metal Body with 120+ Sports Modes, SpO2, Heart Rate Monitoring (Dark Grey)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2,999</t>
+          <t>1499</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1272,17 +1272,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Fire-Boltt</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Fastrack Astor FR2 Pro 1.43" AMOLED Stainless Steel Smart Watch with SpO2, Heart Rate, BT Calling, Adaptive AOD, Functional Crown, AI Voice Assistant – Smartwatch for Stylish Professionals (Black)</t>
+          <t>Fire-Boltt Phoenix Ultra Luxury Stainless Steel, Bluetooth Calling Smart Watch, AI Voice Assistant, Metal Body with 120+ Sports Modes, SpO2, Heart Rate Monitoring (Dark Grey)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2,999</t>
+          <t>1499</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1294,17 +1294,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Titan</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Fastrack Volt S1 Smart Watch for Man and Women Latest with 1.83" Display, Silicone Strap, BT Calling, 100+ Sports Modes, Heart Rate, SpO2, IP68, Ideal Smartwatch for Boys and Girls (Wine Red)</t>
+          <t>Neo Economy Analog White Dial Men's Watch 1802SL08/NN1802SL08/NP1802SL08</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1,499</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1316,17 +1316,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Titan</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Fastrack Volt S1 Smart Watch for Man and Women Latest with 1.83" Display, Silicone Strap, BT Calling, 100+ Sports Modes, Heart Rate, SpO2, IP68, Ideal Smartwatch for Boys and Girls (Wine Red)</t>
+          <t>Neo Economy Analog White Dial Men's Watch 1802SL08/NN1802SL08/NP1802SL08</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1,499</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1338,17 +1338,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Fire-Boltt</t>
+          <t>LORENZ</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Fire-Boltt Phoenix Smart Watch with Bluetooth Calling 1.38,120+ Sports Modes, 240 * 240 PX High Res with SpO2, Heart Rate Monitoring &amp; IP67 Rating (Black)</t>
+          <t>Gift Combo Set for Men | Stylish Steel Analog Watch, PU Leather Wallet &amp; UV Sunglasses | Gift Box for Birthday, Anniversary, Corporate Gifting</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>1,199</t>
+          <t>699</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1360,17 +1360,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Fire-Boltt</t>
+          <t>LORENZ</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Fire-Boltt Phoenix Smart Watch with Bluetooth Calling 1.38,120+ Sports Modes, 240 * 240 PX High Res with SpO2, Heart Rate Monitoring &amp; IP67 Rating (Black)</t>
+          <t>Gift Combo Set for Men | Stylish Steel Analog Watch, PU Leather Wallet &amp; UV Sunglasses | Gift Box for Birthday, Anniversary, Corporate Gifting</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1,199</t>
+          <t>699</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1382,17 +1382,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Fire-Boltt</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Fire-Boltt Phoenix Ultra Luxury Stainless Steel, Bluetooth Calling Smart Watch, AI Voice Assistant, Metal Body with 120+ Sports Modes, SpO2, Heart Rate Monitoring (Dark Grey)</t>
+          <t>Fastrack Analog Grey Dial Men's Watch-FV30004QM01W</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1,499</t>
+          <t>1792</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1404,17 +1404,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Fire-Boltt</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Fire-Boltt Phoenix Ultra Luxury Stainless Steel, Bluetooth Calling Smart Watch, AI Voice Assistant, Metal Body with 120+ Sports Modes, SpO2, Heart Rate Monitoring (Dark Grey)</t>
+          <t>Fastrack Analog Grey Dial Men's Watch-FV30004QM01W</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1,499</t>
+          <t>1792</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1426,17 +1426,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Titan</t>
+          <t>TIMEX</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Neo Economy Analog White Dial Men's Watch 1802SL08/NN1802SL08/NP1802SL08</t>
+          <t>Classics Analog Watch for Men with Round Dial &amp; Water Resistant Man's Wrist Watches</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1,995</t>
+          <t>1193</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1448,17 +1448,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Titan</t>
+          <t>TIMEX</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Neo Economy Analog White Dial Men's Watch 1802SL08/NN1802SL08/NP1802SL08</t>
+          <t>Classics Analog Watch for Men with Round Dial &amp; Water Resistant Man's Wrist Watches</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1,995</t>
+          <t>1193</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1470,17 +1470,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>LORENZ</t>
+          <t>LONGBO</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Gift Combo Set for Men | Stylish Steel Analog Watch, PU Leather Wallet &amp; UV Sunglasses | Gift Box for Birthday, Anniversary, Corporate Gifting</t>
+          <t>Zenith Diamond Analog Watch for Men Business Stainless Steel Watches Luxury Men’s Wristwatch | Birthday Gift for Men | Gift for Husband | Gift for Brother</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>699</t>
+          <t>1690</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1492,17 +1492,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>LORENZ</t>
+          <t>LONGBO</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Gift Combo Set for Men | Stylish Steel Analog Watch, PU Leather Wallet &amp; UV Sunglasses | Gift Box for Birthday, Anniversary, Corporate Gifting</t>
+          <t>Zenith Diamond Analog Watch for Men Business Stainless Steel Watches Luxury Men’s Wristwatch | Birthday Gift for Men | Gift for Husband | Gift for Brother</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>699</t>
+          <t>1690</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1514,17 +1514,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Sonata</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Fastrack Analog Grey Dial Men's Watch-FV30004QM01W</t>
+          <t>Smart Plaid Quartz Analog Black Dial Leather Strap Watch for Men-NS77105SL02W/NT77105SL02W</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1,792</t>
+          <t>1075</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1536,17 +1536,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Sonata</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Fastrack Analog Grey Dial Men's Watch-FV30004QM01W</t>
+          <t>Smart Plaid Quartz Analog Black Dial Leather Strap Watch for Men-NS77105SL02W/NT77105SL02W</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>1,792</t>
+          <t>1075</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1558,17 +1558,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>TIMEX</t>
+          <t>Carlington</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Classics Analog Watch for Men with Round Dial &amp; Water Resistant Man's Wrist Watches</t>
+          <t>Analog-Digital Sports Watch Chronograph, Dual Time,Alarm, Stopwatch, Calendar, Water-Resistant, Shock-Resistant, Back Light Display. The Perfect Watch for Men-CT9140 Series</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1,193</t>
+          <t>1299</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1580,17 +1580,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>TIMEX</t>
+          <t>Carlington</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Classics Analog Watch for Men with Round Dial &amp; Water Resistant Man's Wrist Watches</t>
+          <t>Analog-Digital Sports Watch Chronograph, Dual Time,Alarm, Stopwatch, Calendar, Water-Resistant, Shock-Resistant, Back Light Display. The Perfect Watch for Men-CT9140 Series</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1,193</t>
+          <t>1299</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1602,17 +1602,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>LONGBO</t>
+          <t>Carlington</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Zenith Diamond Analog Watch for Men Business Stainless Steel Watches Luxury Men’s Wristwatch | Birthday Gift for Men | Gift for Husband | Gift for Brother</t>
+          <t>Analog Wrist Watch for Men-CT 8811</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1,690</t>
+          <t>1799</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1624,17 +1624,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>LONGBO</t>
+          <t>Carlington</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Zenith Diamond Analog Watch for Men Business Stainless Steel Watches Luxury Men’s Wristwatch | Birthday Gift for Men | Gift for Husband | Gift for Brother</t>
+          <t>Analog Wrist Watch for Men-CT 8811</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>1,690</t>
+          <t>1799</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1646,17 +1646,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Sonata</t>
+          <t>Carlington</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Smart Plaid Quartz Analog Black Dial Leather Strap Watch for Men-NS77105SL02W/NT77105SL02W</t>
+          <t>Analog Watches for Men with Leather Strap - CT 1050</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1,075</t>
+          <t>999</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1668,17 +1668,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Sonata</t>
+          <t>Carlington</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Smart Plaid Quartz Analog Black Dial Leather Strap Watch for Men-NS77105SL02W/NT77105SL02W</t>
+          <t>Analog Watches for Men with Leather Strap - CT 1050</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1,075</t>
+          <t>999</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1690,17 +1690,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Carlington</t>
+          <t>SKMEI</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Analog-Digital Sports Watch Chronograph, Dual Time,Alarm, Stopwatch, Calendar, Water-Resistant, Shock-Resistant, Back Light Display. The Perfect Watch for Men-CT9140 Series</t>
+          <t>New Car Wheel Watch with Rolling Creative Fashion Analog Watch, Black Dial Zink Alloy Case Men's Watch, Stainless Steel Black Color Band, Quartz Movement, Water &amp; Scratch-Resistant-1990</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1,299</t>
+          <t>1799</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1712,17 +1712,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Carlington</t>
+          <t>SKMEI</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Analog-Digital Sports Watch Chronograph, Dual Time,Alarm, Stopwatch, Calendar, Water-Resistant, Shock-Resistant, Back Light Display. The Perfect Watch for Men-CT9140 Series</t>
+          <t>New Car Wheel Watch with Rolling Creative Fashion Analog Watch, Black Dial Zink Alloy Case Men's Watch, Stainless Steel Black Color Band, Quartz Movement, Water &amp; Scratch-Resistant-1990</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>1,299</t>
+          <t>1799</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1734,17 +1734,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Carlington</t>
+          <t>TIMEWEAR</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Analog Wrist Watch for Men-CT 8811</t>
+          <t>Analog Day Date Functioning Stainless Steel Chain Watch for Men</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>1,799</t>
+          <t>379</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1756,17 +1756,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Carlington</t>
+          <t>TIMEWEAR</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Analog Wrist Watch for Men-CT 8811</t>
+          <t>Analog Day Date Functioning Stainless Steel Chain Watch for Men</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>1,799</t>
+          <t>379</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1778,17 +1778,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Carlington</t>
+          <t>Luminex Commerce</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Analog Watches for Men with Leather Strap - CT 1050</t>
+          <t>Luminex Commerce Men Luxury Fashion Quartz Wrist Watch , Stainless Steel Strap Business Watches For Man, Scratch-Resistant Dial Unique Colorful Analogue Watch, Waterproof Square Wrist Watch - Black</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>999</t>
+          <t>1999</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1800,17 +1800,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Carlington</t>
+          <t>Luminex Commerce</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Analog Watches for Men with Leather Strap - CT 1050</t>
+          <t>Luminex Commerce Men Luxury Fashion Quartz Wrist Watch , Stainless Steel Strap Business Watches For Man, Scratch-Resistant Dial Unique Colorful Analogue Watch, Waterproof Square Wrist Watch - Black</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>999</t>
+          <t>1999</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -1822,17 +1822,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>SKMEI</t>
+          <t>Titan</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>New Car Wheel Watch with Rolling Creative Fashion Analog Watch, Black Dial Zink Alloy Case Men's Watch, Stainless Steel Black Color Band, Quartz Movement, Water &amp; Scratch-Resistant-1990</t>
+          <t>Karishma Analog Black Dial Men's Watch NM1639SM02/NN1639SM02</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>1,799</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -1844,17 +1844,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>SKMEI</t>
+          <t>Titan</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>New Car Wheel Watch with Rolling Creative Fashion Analog Watch, Black Dial Zink Alloy Case Men's Watch, Stainless Steel Black Color Band, Quartz Movement, Water &amp; Scratch-Resistant-1990</t>
+          <t>Karishma Analog Black Dial Men's Watch NM1639SM02/NN1639SM02</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>1,799</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -1866,17 +1866,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>TIMEWEAR</t>
+          <t>Sonata</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Analog Day Date Functioning Stainless Steel Chain Watch for Men</t>
+          <t>Essentials Quartz Analog with Day and Date Forest Green Dial Gold Stainless Steel Strap Watch for Men - NT77082YM05W</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>379</t>
+          <t>1699</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -1888,17 +1888,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>TIMEWEAR</t>
+          <t>Sonata</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Analog Day Date Functioning Stainless Steel Chain Watch for Men</t>
+          <t>Essentials Quartz Analog with Day and Date Forest Green Dial Gold Stainless Steel Strap Watch for Men - NT77082YM05W</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>379</t>
+          <t>1699</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -1910,17 +1910,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Luminex Commerce</t>
+          <t>Boltt</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Luminex Commerce Men Luxury Fashion Quartz Wrist Watch , Stainless Steel Strap Business Watches For Man, Scratch-Resistant Dial Unique Colorful Analogue Watch, Waterproof Square Wrist Watch - Black</t>
+          <t>Boltt Obsidian 33.5mm (1.32 inch) AMOLED Display, Stainless Steel Design, 466 * 466 px Resolution, Bluetooth Calling, Multiple Sports Modes, Health Mode, IP67, Weather Updates</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>1,999</t>
+          <t>1699</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -1932,17 +1932,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Luminex Commerce</t>
+          <t>Boltt</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Luminex Commerce Men Luxury Fashion Quartz Wrist Watch , Stainless Steel Strap Business Watches For Man, Scratch-Resistant Dial Unique Colorful Analogue Watch, Waterproof Square Wrist Watch - Black</t>
+          <t>Boltt Obsidian 33.5mm (1.32 inch) AMOLED Display, Stainless Steel Design, 466 * 466 px Resolution, Bluetooth Calling, Multiple Sports Modes, Health Mode, IP67, Weather Updates</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>1,999</t>
+          <t>1699</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -1954,17 +1954,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Titan</t>
+          <t>Sonata</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Karishma Analog Black Dial Men's Watch NM1639SM02/NN1639SM02</t>
+          <t>Smart Plaid Quartz Analog Black Dial Silver Stainless Steel Strap Watch for Men - NT77105SM02W</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>1,995</t>
+          <t>1185</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -1976,17 +1976,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Titan</t>
+          <t>Sonata</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Karishma Analog Black Dial Men's Watch NM1639SM02/NN1639SM02</t>
+          <t>Smart Plaid Quartz Analog Black Dial Silver Stainless Steel Strap Watch for Men - NT77105SM02W</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>1,995</t>
+          <t>1185</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2003,12 +2003,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Essentials Quartz Analog with Day and Date Forest Green Dial Gold Stainless Steel Strap Watch for Men - NT77082YM05W</t>
+          <t>Volt+ Analog Green Dial Men's Watch NM77085PL02/NN77085PL02W</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>1,699</t>
+          <t>849</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2025,12 +2025,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Essentials Quartz Analog with Day and Date Forest Green Dial Gold Stainless Steel Strap Watch for Men - NT77082YM05W</t>
+          <t>Volt+ Analog Green Dial Men's Watch NM77085PL02/NN77085PL02W</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>1,699</t>
+          <t>849</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2042,17 +2042,17 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Boltt</t>
+          <t>TIMEWEAR</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Boltt Obsidian 33.5mm (1.32 inch) AMOLED Display, Stainless Steel Design, 466 * 466 px Resolution, Bluetooth Calling, Multiple Sports Modes, Health Mode, IP67, Weather Updates</t>
+          <t>Analog, Day Date Functioning, Stainless Steel Chain Watch for Men</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>1,699</t>
+          <t>379</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2064,17 +2064,17 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Boltt</t>
+          <t>TIMEWEAR</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Boltt Obsidian 33.5mm (1.32 inch) AMOLED Display, Stainless Steel Design, 466 * 466 px Resolution, Bluetooth Calling, Multiple Sports Modes, Health Mode, IP67, Weather Updates</t>
+          <t>Analog, Day Date Functioning, Stainless Steel Chain Watch for Men</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>1,699</t>
+          <t>379</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2086,17 +2086,17 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Sonata</t>
+          <t>SKMEI</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Smart Plaid Quartz Analog Black Dial Silver Stainless Steel Strap Watch for Men - NT77105SM02W</t>
+          <t>Men's Spinning Car Wheels Rolling Creative Fashion Watches for Men, Analog Watch Black Dial Zink Alloy Case Men's Watch, Black Color Stainless Steel Band, Rolling Wheel Gift Wristwatch - 1787</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>1,185</t>
+          <t>1799</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2108,17 +2108,17 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Sonata</t>
+          <t>SKMEI</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Smart Plaid Quartz Analog Black Dial Silver Stainless Steel Strap Watch for Men - NT77105SM02W</t>
+          <t>Men's Spinning Car Wheels Rolling Creative Fashion Watches for Men, Analog Watch Black Dial Zink Alloy Case Men's Watch, Black Color Stainless Steel Band, Rolling Wheel Gift Wristwatch - 1787</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>1,185</t>
+          <t>1799</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2130,17 +2130,17 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Sonata</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Volt+ Analog Green Dial Men's Watch NM77085PL02/NN77085PL02W</t>
+          <t>Analog Unisex-Adult Watch</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>849</t>
+          <t>895</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2152,17 +2152,17 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Sonata</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Volt+ Analog Green Dial Men's Watch NM77085PL02/NN77085PL02W</t>
+          <t>Analog Unisex-Adult Watch</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>849</t>
+          <t>895</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2174,17 +2174,17 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>TIMEWEAR</t>
+          <t>boAt</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Analog, Day Date Functioning, Stainless Steel Chain Watch for Men</t>
+          <t>boAt Lunar Discovery w/ 1.39" (3.5 cm) HD Display, Turn-by-Turn Navigation, DIY Watch Face Studio, Bluetooth Calling, Emergency SOS, QR Tray, Smart Watch for Men &amp; Women(Brown)</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>379</t>
+          <t>1499</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2196,17 +2196,17 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>TIMEWEAR</t>
+          <t>boAt</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Analog, Day Date Functioning, Stainless Steel Chain Watch for Men</t>
+          <t>boAt Lunar Discovery w/ 1.39" (3.5 cm) HD Display, Turn-by-Turn Navigation, DIY Watch Face Studio, Bluetooth Calling, Emergency SOS, QR Tray, Smart Watch for Men &amp; Women(Brown)</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>379</t>
+          <t>1499</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2218,17 +2218,17 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>SKMEI</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Men's Spinning Car Wheels Rolling Creative Fashion Watches for Men, Analog Watch Black Dial Zink Alloy Case Men's Watch, Black Color Stainless Steel Band, Rolling Wheel Gift Wristwatch - 1787</t>
+          <t>Casual Analog Black Dial Men's Watch NM3121SM02/NN3121SM02</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>1,799</t>
+          <t>1895</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2240,17 +2240,17 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>SKMEI</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Men's Spinning Car Wheels Rolling Creative Fashion Watches for Men, Analog Watch Black Dial Zink Alloy Case Men's Watch, Black Color Stainless Steel Band, Rolling Wheel Gift Wristwatch - 1787</t>
+          <t>Casual Analog Black Dial Men's Watch NM3121SM02/NN3121SM02</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>1,799</t>
+          <t>1895</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2262,17 +2262,17 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>TIMEX</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Analog Unisex-Adult Watch</t>
+          <t>TIMEX Analog Watch for Man with Blue Round Dial &amp; Multicolor Stainless Steel Bracelet Band Water Resistant Men's Wrist Watches - TWTG73SMU03</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>895</t>
+          <t>1557</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2284,17 +2284,17 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>TIMEX</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Analog Unisex-Adult Watch</t>
+          <t>TIMEX Analog Watch for Man with Blue Round Dial &amp; Multicolor Stainless Steel Bracelet Band Water Resistant Men's Wrist Watches - TWTG73SMU03</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>895</t>
+          <t>1557</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2306,17 +2306,17 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>boAt</t>
+          <t>TIMEX</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>boAt Lunar Discovery w/ 1.39" (3.5 cm) HD Display, Turn-by-Turn Navigation, DIY Watch Face Studio, Bluetooth Calling, Emergency SOS, QR Tray, Smart Watch for Men &amp; Women(Brown)</t>
+          <t>Classics Analog Watch for Men with Round Dial &amp; Water Resistant Man's Wrist Watches</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>1,499</t>
+          <t>1829</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2328,17 +2328,17 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>boAt</t>
+          <t>TIMEX</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>boAt Lunar Discovery w/ 1.39" (3.5 cm) HD Display, Turn-by-Turn Navigation, DIY Watch Face Studio, Bluetooth Calling, Emergency SOS, QR Tray, Smart Watch for Men &amp; Women(Brown)</t>
+          <t>Classics Analog Watch for Men with Round Dial &amp; Water Resistant Man's Wrist Watches</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>1,499</t>
+          <t>1829</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2350,17 +2350,17 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Carlington</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Casual Analog Black Dial Men's Watch NM3121SM02/NN3121SM02</t>
+          <t>Legacy Series Analog Wrist Watches with Chronograph &amp; Silicone Strap for Men - CT 9999</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>1,895</t>
+          <t>1499</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2372,17 +2372,17 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Carlington</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Casual Analog Black Dial Men's Watch NM3121SM02/NN3121SM02</t>
+          <t>Legacy Series Analog Wrist Watches with Chronograph &amp; Silicone Strap for Men - CT 9999</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>1,895</t>
+          <t>1499</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2394,17 +2394,17 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>TIMEX</t>
+          <t>Fire-Boltt</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>TIMEX Analog Watch for Man with Blue Round Dial &amp; Multicolor Stainless Steel Bracelet Band Water Resistant Men's Wrist Watches - TWTG73SMU03</t>
+          <t>Fire-Boltt Ninja Call Pro Max Ultra Smart Watch 2.01 inch Display, Bluetooth Calling, 120+ Sports Modes, Health Suite, Voice Assistance (Black SS)</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>1,557</t>
+          <t>1099</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2416,17 +2416,17 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>TIMEX</t>
+          <t>Fire-Boltt</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>TIMEX Analog Watch for Man with Blue Round Dial &amp; Multicolor Stainless Steel Bracelet Band Water Resistant Men's Wrist Watches - TWTG73SMU03</t>
+          <t>Fire-Boltt Ninja Call Pro Max Ultra Smart Watch 2.01 inch Display, Bluetooth Calling, 120+ Sports Modes, Health Suite, Voice Assistance (Black SS)</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>1,557</t>
+          <t>1099</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2438,17 +2438,17 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>TIMEX</t>
+          <t>Sonata</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Classics Analog Watch for Men with Round Dial &amp; Water Resistant Man's Wrist Watches</t>
+          <t>Essentials Quartz Analog Black Dial Silver Stainless Steel Strap Watch for Men - NS77083SM05W</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>1,829</t>
+          <t>949</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2460,17 +2460,17 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>TIMEX</t>
+          <t>Sonata</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Classics Analog Watch for Men with Round Dial &amp; Water Resistant Man's Wrist Watches</t>
+          <t>Essentials Quartz Analog Black Dial Silver Stainless Steel Strap Watch for Men - NS77083SM05W</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>1,829</t>
+          <t>949</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2482,17 +2482,17 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Carlington</t>
+          <t>LOUIS DEVIN</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Legacy Series Analog Wrist Watches with Chronograph &amp; Silicone Strap for Men - CT 9999</t>
+          <t>Silicone Strap Analog Wrist Watch for Men (Black/Blue/Red) | LD-BK054</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>1,499</t>
+          <t>369</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2504,17 +2504,17 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Carlington</t>
+          <t>LOUIS DEVIN</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Legacy Series Analog Wrist Watches with Chronograph &amp; Silicone Strap for Men - CT 9999</t>
+          <t>Silicone Strap Analog Wrist Watch for Men (Black/Blue/Red) | LD-BK054</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>1,499</t>
+          <t>369</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2526,17 +2526,17 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Fire-Boltt</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Fire-Boltt Ninja Call Pro Max Ultra Smart Watch 2.01 inch Display, Bluetooth Calling, 120+ Sports Modes, Health Suite, Voice Assistance (Black SS)</t>
+          <t>Men Stunners Quartz Analog Grey Dial Brown Leather Strap Watch for Guys - NR3291SL01?</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>1,099</t>
+          <t>1495</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2548,17 +2548,17 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Fire-Boltt</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Fire-Boltt Ninja Call Pro Max Ultra Smart Watch 2.01 inch Display, Bluetooth Calling, 120+ Sports Modes, Health Suite, Voice Assistance (Black SS)</t>
+          <t>Men Stunners Quartz Analog Grey Dial Brown Leather Strap Watch for Guys - NR3291SL01?</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>1,099</t>
+          <t>1495</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2570,17 +2570,17 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Sonata</t>
+          <t>Noise</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Essentials Quartz Analog Black Dial Silver Stainless Steel Strap Watch for Men - NS77083SM05W</t>
+          <t>Noise Twist Go Smart Watch 1.39" Display, TruSyncᵀᴹ BT Calling, Glossy Metal Finish, 150+ Watch Faces, IP68, Sleep Tracking, 100+ Sports Modes, Smart Watch for Men and Women (Silver Blue)</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>949</t>
+          <t>1399</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -2592,17 +2592,17 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Sonata</t>
+          <t>Noise</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Essentials Quartz Analog Black Dial Silver Stainless Steel Strap Watch for Men - NS77083SM05W</t>
+          <t>Noise Twist Go Smart Watch 1.39" Display, TruSyncᵀᴹ BT Calling, Glossy Metal Finish, 150+ Watch Faces, IP68, Sleep Tracking, 100+ Sports Modes, Smart Watch for Men and Women (Silver Blue)</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>949</t>
+          <t>1399</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -2614,17 +2614,17 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>LOUIS DEVIN</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Silicone Strap Analog Wrist Watch for Men (Black/Blue/Red) | LD-BK054</t>
+          <t>Fastrack Volt S1 Smart Watch for Man and Women Latest with 1.83" Display, Silicone Strap, BT Calling, 100+ Sports Modes, Heart Rate, SpO2, IP68, Ideal Smartwatch for Boys and Girls (Black)</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>369</t>
+          <t>1499</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -2636,17 +2636,17 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>LOUIS DEVIN</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Silicone Strap Analog Wrist Watch for Men (Black/Blue/Red) | LD-BK054</t>
+          <t>Fastrack Volt S1 Smart Watch for Man and Women Latest with 1.83" Display, Silicone Strap, BT Calling, 100+ Sports Modes, Heart Rate, SpO2, IP68, Ideal Smartwatch for Boys and Girls (Black)</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>369</t>
+          <t>1499</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -2658,17 +2658,17 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Sonata</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Men Stunners Quartz Analog Grey Dial Brown Leather Strap Watch for Guys - NR3291SL01?</t>
+          <t>SF Quartz Analog White Dial Black Plastic Strap Watch for Men- NT7930PP01</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>1,495</t>
+          <t>675</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -2680,17 +2680,17 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Sonata</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Men Stunners Quartz Analog Grey Dial Brown Leather Strap Watch for Guys - NR3291SL01?</t>
+          <t>SF Quartz Analog White Dial Black Plastic Strap Watch for Men- NT7930PP01</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>1,495</t>
+          <t>675</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -2702,17 +2702,17 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Noise</t>
+          <t>Fire-Boltt</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Noise Twist Go Smart Watch 1.39" Display, TruSyncᵀᴹ BT Calling, Glossy Metal Finish, 150+ Watch Faces, IP68, Sleep Tracking, 100+ Sports Modes, Smart Watch for Men and Women (Silver Blue)</t>
+          <t>Fire-Boltt Newly Launched Phoenix Ultra Blaze Luxury Stainless Steel, Bluetooth Calling Smart Watch, AI Voice Assistant, Metal Body with 120+ Sports Modes, SpO2, Heart Rate Monitoring (Silver)</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>1,399</t>
+          <t>1799</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -2724,17 +2724,17 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Noise</t>
+          <t>Fire-Boltt</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Noise Twist Go Smart Watch 1.39" Display, TruSyncᵀᴹ BT Calling, Glossy Metal Finish, 150+ Watch Faces, IP68, Sleep Tracking, 100+ Sports Modes, Smart Watch for Men and Women (Silver Blue)</t>
+          <t>Fire-Boltt Newly Launched Phoenix Ultra Blaze Luxury Stainless Steel, Bluetooth Calling Smart Watch, AI Voice Assistant, Metal Body with 120+ Sports Modes, SpO2, Heart Rate Monitoring (Silver)</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>1,399</t>
+          <t>1799</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -2746,17 +2746,17 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>SKMEI</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Fastrack Volt S1 Smart Watch for Man and Women Latest with 1.83" Display, Silicone Strap, BT Calling, 100+ Sports Modes, Heart Rate, SpO2, IP68, Ideal Smartwatch for Boys and Girls (Black)</t>
+          <t>Men's Digital Sports Watch 50m Waterproof LED Military Multifunction Smart Watch Stopwatch Countdown Auto Date Alarm</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>1,499</t>
+          <t>699</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -2768,17 +2768,17 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>SKMEI</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Fastrack Volt S1 Smart Watch for Man and Women Latest with 1.83" Display, Silicone Strap, BT Calling, 100+ Sports Modes, Heart Rate, SpO2, IP68, Ideal Smartwatch for Boys and Girls (Black)</t>
+          <t>Men's Digital Sports Watch 50m Waterproof LED Military Multifunction Smart Watch Stopwatch Countdown Auto Date Alarm</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>1,499</t>
+          <t>699</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -2790,17 +2790,17 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Sonata</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>SF Quartz Analog White Dial Black Plastic Strap Watch for Men- NT7930PP01</t>
+          <t>Fastrack Vyb Quartz Analog Silver Dial Steel Sheet Metal Strap Watch for Men-FV30014SM01W</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>675</t>
+          <t>1665</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -2812,17 +2812,17 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Sonata</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>SF Quartz Analog White Dial Black Plastic Strap Watch for Men- NT7930PP01</t>
+          <t>Fastrack Vyb Quartz Analog Silver Dial Steel Sheet Metal Strap Watch for Men-FV30014SM01W</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>675</t>
+          <t>1665</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -2834,17 +2834,17 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Fire-Boltt</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Fire-Boltt Newly Launched Phoenix Ultra Blaze Luxury Stainless Steel, Bluetooth Calling Smart Watch, AI Voice Assistant, Metal Body with 120+ Sports Modes, SpO2, Heart Rate Monitoring (Silver)</t>
+          <t>Stunners Quartz Analog Silver Dial Silver Metal Strap Watch for Guys - NT3291SM02​</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>1,799</t>
+          <t>1795</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -2856,17 +2856,17 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Fire-Boltt</t>
+          <t>Fastrack</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Fire-Boltt Newly Launched Phoenix Ultra Blaze Luxury Stainless Steel, Bluetooth Calling Smart Watch, AI Voice Assistant, Metal Body with 120+ Sports Modes, SpO2, Heart Rate Monitoring (Silver)</t>
+          <t>Stunners Quartz Analog Silver Dial Silver Metal Strap Watch for Guys - NT3291SM02​</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>1,799</t>
+          <t>1795</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -2878,17 +2878,17 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>SKMEI</t>
+          <t>Titan</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Men's Digital Sports Watch 50m Waterproof LED Military Multifunction Smart Watch Stopwatch Countdown Auto Date Alarm</t>
+          <t>Karishma Analog Black Dial Men's Watch NM1639SM02/NN1639SM02</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>699</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -2900,17 +2900,17 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>SKMEI</t>
+          <t>Titan</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Men's Digital Sports Watch 50m Waterproof LED Military Multifunction Smart Watch Stopwatch Countdown Auto Date Alarm</t>
+          <t>Karishma Analog Black Dial Men's Watch NM1639SM02/NN1639SM02</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>699</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -2922,17 +2922,17 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Titan</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Fastrack Vyb Quartz Analog Silver Dial Steel Sheet Metal Strap Watch for Men-FV30014SM01W</t>
+          <t>Titan Neo Iv Analog Silver Dial Men's Watch-1802SL02 / 1802SL02</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>1,665.</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -2944,17 +2944,17 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Titan</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Fastrack Vyb Quartz Analog Silver Dial Steel Sheet Metal Strap Watch for Men-FV30014SM01W</t>
+          <t>Titan Neo Iv Analog Silver Dial Men's Watch-1802SL02 / 1802SL02</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>1,665.</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -2966,17 +2966,17 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Carlington</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Stunners Quartz Analog Silver Dial Silver Metal Strap Watch for Guys - NT3291SM02​</t>
+          <t>Analog Wrist Watch for Men-CT 8811</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>1,795</t>
+          <t>1799</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -2988,17 +2988,17 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Carlington</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Stunners Quartz Analog Silver Dial Silver Metal Strap Watch for Guys - NT3291SM02​</t>
+          <t>Analog Wrist Watch for Men-CT 8811</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>1,795</t>
+          <t>1799</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3010,17 +3010,17 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Carlington</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Fastrack Dezire FX1 PRO Fashion Smart Watch, 1.43" AMOLED, 466 * 466 Resolution, SingleSync BT Calling, AI Voice Assistant, 100+ Sports Modes &amp; Smartwatch Faces, Upto 5 Day Battery, IP68 (Rose Gold)</t>
+          <t>Resin Analog-Digital Sports Watch Chronograph,Dual Time,Alarm,Stopwatch,Water-Resistant,Shock-Resistant,Back Light Display- The Perfect Watch for Men&amp;Boys-CT 9107 Series</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>3,499</t>
+          <t>1399</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3032,17 +3032,17 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Carlington</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Fastrack Dezire FX1 PRO Fashion Smart Watch, 1.43" AMOLED, 466 * 466 Resolution, SingleSync BT Calling, AI Voice Assistant, 100+ Sports Modes &amp; Smartwatch Faces, Upto 5 Day Battery, IP68 (Rose Gold)</t>
+          <t>Resin Analog-Digital Sports Watch Chronograph,Dual Time,Alarm,Stopwatch,Water-Resistant,Shock-Resistant,Back Light Display- The Perfect Watch for Men&amp;Boys-CT 9107 Series</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>3,499</t>
+          <t>1399</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -3054,17 +3054,17 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Titan</t>
+          <t>Sonata</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Karishma Analog Black Dial Men's Watch NM1639SM02/NN1639SM02</t>
+          <t>Force Quartz Analog with Day and Date Blue Dial Black Stainless Steel Strap Watch for Men - NT7146NM01</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>1,995</t>
+          <t>1999</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -3076,17 +3076,17 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Titan</t>
+          <t>Sonata</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Karishma Analog Black Dial Men's Watch NM1639SM02/NN1639SM02</t>
+          <t>Force Quartz Analog with Day and Date Blue Dial Black Stainless Steel Strap Watch for Men - NT7146NM01</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>1,995</t>
+          <t>1999</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -3098,17 +3098,17 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Titan</t>
+          <t>Carlington</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Titan Neo Iv Analog Silver Dial Men's Watch-1802SL02 / 1802SL02</t>
+          <t>Premium Watch for Men with Black Colored Chain Watch for Men Stainless Steel and Scratch Resistance</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>1,995</t>
+          <t>999</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -3120,17 +3120,17 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Titan</t>
+          <t>Carlington</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Titan Neo Iv Analog Silver Dial Men's Watch-1802SL02 / 1802SL02</t>
+          <t>Premium Watch for Men with Black Colored Chain Watch for Men Stainless Steel and Scratch Resistance</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>1,995</t>
+          <t>999</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3142,17 +3142,17 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Titan</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Fastrack Radiant FX4 1.51" AMOLED Metal Smart Watch with Single Sync BT Calling, Functional Crown, All-Round Health Tracking, 100+ Sports Modes, IP68 – Smartwatch for Man &amp; Woman (Silver)</t>
+          <t>Karishma Analog Black Dial Men's Watch NM1639SM02/NN1639SM02</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>5,499</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -3164,17 +3164,17 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Fastrack</t>
+          <t>Titan</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Fastrack Radiant FX4 1.51" AMOLED Metal Smart Watch with Single Sync BT Calling, Functional Crown, All-Round Health Tracking, 100+ Sports Modes, IP68 – Smartwatch for Man &amp; Woman (Silver)</t>
+          <t>Karishma Analog Black Dial Men's Watch NM1639SM02/NN1639SM02</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>5,499</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -3186,17 +3186,17 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Tommy Hilfiger</t>
+          <t>Titan</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Quartz Multifunction White Dial Silicone Strap Watch for Men-NETH1791353</t>
+          <t>Neo Economy Analog White Dial Men's Watch 1802SL08/NN1802SL08/NP1802SL08</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>11,425</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -3208,328 +3208,20 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Tommy Hilfiger</t>
+          <t>Titan</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Quartz Multifunction White Dial Silicone Strap Watch for Men-NETH1791353</t>
+          <t>Neo Economy Analog White Dial Men's Watch 1802SL08/NN1802SL08/NP1802SL08</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>11,425</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>Carlington</t>
-        </is>
-      </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>Analog Wrist Watch for Men-CT 8811</t>
-        </is>
-      </c>
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>1,799</t>
-        </is>
-      </c>
-      <c r="D128" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="inlineStr">
-        <is>
-          <t>Carlington</t>
-        </is>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>Analog Wrist Watch for Men-CT 8811</t>
-        </is>
-      </c>
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>1,799</t>
-        </is>
-      </c>
-      <c r="D129" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="inlineStr">
-        <is>
-          <t>Carlington</t>
-        </is>
-      </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>Resin Analog-Digital Sports Watch Chronograph,Dual Time,Alarm,Stopwatch,Water-Resistant,Shock-Resistant,Back Light Display- The Perfect Watch for Men&amp;Boys-CT 9107 Series</t>
-        </is>
-      </c>
-      <c r="C130" t="inlineStr">
-        <is>
-          <t>1,399</t>
-        </is>
-      </c>
-      <c r="D130" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="inlineStr">
-        <is>
-          <t>Carlington</t>
-        </is>
-      </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>Resin Analog-Digital Sports Watch Chronograph,Dual Time,Alarm,Stopwatch,Water-Resistant,Shock-Resistant,Back Light Display- The Perfect Watch for Men&amp;Boys-CT 9107 Series</t>
-        </is>
-      </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>1,399</t>
-        </is>
-      </c>
-      <c r="D131" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="inlineStr">
-        <is>
-          <t>Sonata</t>
-        </is>
-      </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>Force Quartz Analog with Day and Date Blue Dial Black Stainless Steel Strap Watch for Men - NT7146NM01</t>
-        </is>
-      </c>
-      <c r="C132" t="inlineStr">
-        <is>
-          <t>1,999</t>
-        </is>
-      </c>
-      <c r="D132" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="inlineStr">
-        <is>
-          <t>Sonata</t>
-        </is>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>Force Quartz Analog with Day and Date Blue Dial Black Stainless Steel Strap Watch for Men - NT7146NM01</t>
-        </is>
-      </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>1,999</t>
-        </is>
-      </c>
-      <c r="D133" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>Sonata</t>
-        </is>
-      </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>Sonata Quartz Analog with Date White Dial Leather Strap Watch for Couple-NS71338164WL01P</t>
-        </is>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>2,637</t>
-        </is>
-      </c>
-      <c r="D134" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>Sonata</t>
-        </is>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>Sonata Quartz Analog with Date White Dial Leather Strap Watch for Couple-NS71338164WL01P</t>
-        </is>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>2,637</t>
-        </is>
-      </c>
-      <c r="D135" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="inlineStr">
-        <is>
-          <t>Carlington</t>
-        </is>
-      </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>Premium Watch for Men with Black Colored Chain Watch for Men Stainless Steel and Scratch Resistance</t>
-        </is>
-      </c>
-      <c r="C136" t="inlineStr">
-        <is>
-          <t>999</t>
-        </is>
-      </c>
-      <c r="D136" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" t="inlineStr">
-        <is>
-          <t>Carlington</t>
-        </is>
-      </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>Premium Watch for Men with Black Colored Chain Watch for Men Stainless Steel and Scratch Resistance</t>
-        </is>
-      </c>
-      <c r="C137" t="inlineStr">
-        <is>
-          <t>999</t>
-        </is>
-      </c>
-      <c r="D137" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" t="inlineStr">
-        <is>
-          <t>Titan</t>
-        </is>
-      </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>Karishma Analog Black Dial Men's Watch NM1639SM02/NN1639SM02</t>
-        </is>
-      </c>
-      <c r="C138" t="inlineStr">
-        <is>
-          <t>1,995</t>
-        </is>
-      </c>
-      <c r="D138" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" t="inlineStr">
-        <is>
-          <t>Titan</t>
-        </is>
-      </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>Karishma Analog Black Dial Men's Watch NM1639SM02/NN1639SM02</t>
-        </is>
-      </c>
-      <c r="C139" t="inlineStr">
-        <is>
-          <t>1,995</t>
-        </is>
-      </c>
-      <c r="D139" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" t="inlineStr">
-        <is>
-          <t>Titan</t>
-        </is>
-      </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>Neo Economy Analog White Dial Men's Watch 1802SL08/NN1802SL08/NP1802SL08</t>
-        </is>
-      </c>
-      <c r="C140" t="inlineStr">
-        <is>
-          <t>1,995</t>
-        </is>
-      </c>
-      <c r="D140" t="inlineStr">
-        <is>
-          <t>In Stock</t>
-        </is>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" t="inlineStr">
-        <is>
-          <t>Titan</t>
-        </is>
-      </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>Neo Economy Analog White Dial Men's Watch 1802SL08/NN1802SL08/NP1802SL08</t>
-        </is>
-      </c>
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>1,995</t>
-        </is>
-      </c>
-      <c r="D141" t="inlineStr">
         <is>
           <t>In Stock</t>
         </is>

</xml_diff>